<commit_message>
add last added films retrievall
</commit_message>
<xml_diff>
--- a/dvdtheque-rest-services/src/test/resources/ListeDVD.xlsx
+++ b/dvdtheque-rest-services/src/test/resources/ListeDVD.xlsx
@@ -99,22 +99,32 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>Date insertion</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>Zonedvd</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Rippé</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>RIP Date</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Dvd Format</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Date Sortie DVD</t>
         </is>
       </c>
     </row>
@@ -141,7 +151,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>DVD</t>
+          <t>EN_SALLE</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -156,22 +166,32 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10/01/2020</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>oui</t>
+          <t/>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>23/07/2019</t>
+          <t/>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>DVD</t>
+          <t/>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>31/07/0022</t>
         </is>
       </c>
     </row>
@@ -213,22 +233,32 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>10/01/2020</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t/>
+          <t>non</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>DVD</t>
+          <t/>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>
@@ -270,22 +300,32 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>10/01/2020</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t/>
+          <t>oui</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>DVD</t>
+          <t>06/05/2019</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>
@@ -302,7 +342,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -327,22 +367,32 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>10/01/2020</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t/>
+          <t>oui</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>DVD</t>
+          <t>23/07/2019</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>
@@ -359,7 +409,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -384,22 +434,32 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>10/01/2020</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t/>
+          <t>non</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>DVD</t>
+          <t/>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>
@@ -441,22 +501,32 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>10/01/2020</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t/>
+          <t>non</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>DVD</t>
+          <t/>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>
@@ -498,22 +568,32 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>10/01/2020</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t/>
+          <t>non</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>DVD</t>
+          <t/>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>

</xml_diff>